<commit_message>
changed sb csv excel to cut spaces
</commit_message>
<xml_diff>
--- a/merged_SppList_Prop_AI08072022.xlsx
+++ b/merged_SppList_Prop_AI08072022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alissaiverson/.ssh/HLC_soil_and_veg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11575602-F197-3D4C-9E01-863593A35394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FEFFBC-53C8-6B47-B5F1-D693B671A62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -890,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A3" zoomScale="140" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3755,9 +3755,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8F9A7C-1BA1-384E-B8F0-B8493D259D10}">
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="7">
         <v>9.2071610000000002E-3</v>
@@ -5500,7 +5500,7 @@
       <c r="E64" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G64" s="3" t="s">
@@ -5528,7 +5528,7 @@
       <c r="E65" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="F65" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G65" s="3" t="s">
@@ -6362,7 +6362,7 @@
       <c r="E96" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F96" s="3" t="s">
+      <c r="F96" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G96" s="3" t="s">
@@ -6390,7 +6390,7 @@
       <c r="E97" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F97" s="3" t="s">
+      <c r="F97" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G97" s="3" t="s">
@@ -9756,7 +9756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0896B1E9-7AD5-6442-BB4B-BA08182D78D5}">
   <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>